<commit_message>
Skip rows that have "?" in the form column
</commit_message>
<xml_diff>
--- a/test/data/excel/test_single_excel_maweti.xlsx
+++ b/test/data/excel/test_single_excel_maweti.xlsx
@@ -360,13 +360,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25"/>
   </cols>
@@ -497,25 +497,27 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -539,7 +541,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>